<commit_message>
1484.Group Sold Products By The Date
</commit_message>
<xml_diff>
--- a/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
+++ b/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="79">
   <si>
     <t>Easy</t>
   </si>
@@ -893,8 +893,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1871,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="24.95" hidden="1" customHeight="1">
+    <row r="65" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A65" s="7">
         <v>1468</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="24.95" customHeight="1">
+    <row r="66" spans="1:4" ht="24.95" customHeight="1">
       <c r="A66" s="7">
         <v>1484</v>
       </c>
@@ -1892,8 +1892,11 @@
       <c r="C66" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="24.95" customHeight="1">
+      <c r="D66" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="24.95" customHeight="1">
       <c r="A67" s="7">
         <v>1495</v>
       </c>
@@ -1904,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="24.95" hidden="1" customHeight="1">
+    <row r="68" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A68" s="7">
         <v>1501</v>
       </c>
@@ -1915,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="24.95" customHeight="1">
+    <row r="69" spans="1:4" ht="24.95" customHeight="1">
       <c r="A69" s="7">
         <v>1511</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="24.95" customHeight="1">
+    <row r="70" spans="1:4" ht="24.95" customHeight="1">
       <c r="A70" s="7">
         <v>1517</v>
       </c>
@@ -1937,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="24.95" hidden="1" customHeight="1">
+    <row r="71" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A71" s="7">
         <v>1532</v>
       </c>

</xml_diff>

<commit_message>
1517.Find Users With Valid E-Mails
</commit_message>
<xml_diff>
--- a/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
+++ b/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="79">
   <si>
     <t>Easy</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>Countries You Can Safely Invest In    </t>
-  </si>
-  <si>
-    <t>Customer Order Frequency    </t>
   </si>
   <si>
     <t>Find Users With Valid E-Mails    </t>
@@ -372,6 +369,10 @@
   </si>
   <si>
     <t>V</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer Order Frequency    </t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -893,8 +894,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -906,13 +907,13 @@
   <sheetData>
     <row r="1" spans="1:19" ht="24.95" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="24.95" customHeight="1">
@@ -920,16 +921,16 @@
         <v>511</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -957,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -983,7 +984,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -1110,13 +1111,13 @@
         <v>586</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -1139,13 +1140,13 @@
         <v>603</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -1174,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -1229,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
@@ -1258,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="24.95" hidden="1" customHeight="1">
@@ -1294,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="24.95" customHeight="1">
@@ -1308,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="24.95" customHeight="1">
@@ -1322,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="24.95" customHeight="1">
@@ -1336,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1361,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="24.95" customHeight="1">
@@ -1375,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="24.95" customHeight="1">
@@ -1389,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1436,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1472,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="24.95" customHeight="1">
@@ -1486,7 +1487,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1522,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1602,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1638,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1663,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="24.95" customHeight="1">
@@ -1677,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1713,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="24.95" customHeight="1">
@@ -1727,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1763,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1788,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1824,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1893,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="24.95" customHeight="1">
@@ -1906,6 +1907,9 @@
       <c r="C67" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D67" s="12" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="68" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A68" s="7">
@@ -1923,10 +1927,13 @@
         <v>1511</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>0</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="24.95" customHeight="1">
@@ -1934,10 +1941,13 @@
         <v>1517</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>0</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1945,7 +1955,7 @@
         <v>1532</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
1149.Article Views II 文章瀏灠量
</commit_message>
<xml_diff>
--- a/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
+++ b/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="80">
   <si>
     <t>Easy</t>
   </si>
@@ -911,8 +911,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1494,6 +1494,9 @@
       <c r="C29" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="D29" s="13" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="24.95" customHeight="1">
       <c r="A30" s="7">
@@ -1505,6 +1508,9 @@
       <c r="C30" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="D30" s="13" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A31" s="7">
@@ -1543,6 +1549,9 @@
       </c>
       <c r="C33" s="10" t="s">
         <v>1</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="24.95" customHeight="1">

</xml_diff>

<commit_message>
1164.Product Price at a Given Date 給定日期的產品價格
</commit_message>
<xml_diff>
--- a/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
+++ b/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="80">
   <si>
     <t>Easy</t>
   </si>
@@ -911,8 +911,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1563,6 +1563,9 @@
       </c>
       <c r="C34" s="10" t="s">
         <v>1</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="24.95" hidden="1" customHeight="1">

</xml_diff>

<commit_message>
1440.Evaluate Boolean Expression 計算布林表達式的值
</commit_message>
<xml_diff>
--- a/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
+++ b/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="80">
   <si>
     <t>Easy</t>
   </si>
@@ -602,11 +602,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -914,7 +914,7 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -948,23 +948,23 @@
       <c r="D2" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
     </row>
     <row r="3" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A3" s="7">
@@ -979,21 +979,21 @@
       <c r="D3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
     </row>
     <row r="4" spans="1:19" ht="24.95" customHeight="1">
       <c r="A4" s="7">
@@ -1002,27 +1002,27 @@
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>79</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:19" ht="24.95" customHeight="1">
       <c r="A5" s="7">
@@ -1031,27 +1031,27 @@
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
     </row>
     <row r="6" spans="1:19" ht="24.95" customHeight="1">
       <c r="A6" s="7">
@@ -1060,27 +1060,27 @@
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A7" s="7">
@@ -1092,21 +1092,21 @@
       <c r="C7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
     </row>
     <row r="8" spans="1:19" ht="24.95" customHeight="1">
       <c r="A8" s="7">
@@ -1115,27 +1115,27 @@
       <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
     </row>
     <row r="9" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A9" s="7">
@@ -1150,21 +1150,21 @@
       <c r="D9" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
     </row>
     <row r="10" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A10" s="7">
@@ -1179,21 +1179,21 @@
       <c r="D10" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
     </row>
     <row r="11" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A11" s="7">
@@ -1208,21 +1208,21 @@
       <c r="D11" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
     </row>
     <row r="12" spans="1:19" ht="24.95" customHeight="1">
       <c r="A12" s="7">
@@ -1231,27 +1231,27 @@
       <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
     </row>
     <row r="13" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A13" s="7">
@@ -1266,21 +1266,21 @@
       <c r="D13" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
     </row>
     <row r="14" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A14" s="7">
@@ -1314,7 +1314,7 @@
       <c r="B16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -1384,7 +1384,7 @@
       <c r="B21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="12" t="s">
@@ -1451,7 +1451,7 @@
       <c r="B26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="12" t="s">
@@ -1465,7 +1465,7 @@
       <c r="B27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="12" t="s">
@@ -1493,7 +1493,7 @@
       <c r="B29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="12" t="s">
@@ -1507,7 +1507,7 @@
       <c r="B30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="12" t="s">
@@ -1549,7 +1549,7 @@
       <c r="B33" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="12" t="s">
@@ -1563,7 +1563,7 @@
       <c r="B34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="12" t="s">
@@ -1591,7 +1591,7 @@
       <c r="B36" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="12" t="s">
@@ -1616,7 +1616,7 @@
       <c r="B38" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D38" s="12" t="s">
@@ -1630,7 +1630,7 @@
       <c r="B39" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="12" t="s">
@@ -1644,7 +1644,7 @@
       <c r="B40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D40" s="12" t="s">
@@ -1683,7 +1683,7 @@
       <c r="B43" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="12" t="s">
@@ -1697,7 +1697,7 @@
       <c r="B44" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="12" t="s">
@@ -1725,7 +1725,7 @@
       <c r="B46" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="12" t="s">
@@ -1767,7 +1767,7 @@
       <c r="B49" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D49" s="12" t="s">
@@ -1781,7 +1781,7 @@
       <c r="B50" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="12" t="s">
@@ -1834,7 +1834,7 @@
       <c r="B54" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D54" s="12" t="s">
@@ -1898,8 +1898,11 @@
       <c r="B59" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="14" t="s">
-        <v>1</v>
+      <c r="C59" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="24.95" hidden="1" customHeight="1">
@@ -1948,8 +1951,11 @@
       <c r="B63" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="14" t="s">
-        <v>1</v>
+      <c r="C63" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="24.95" customHeight="1">
@@ -1959,7 +1965,7 @@
       <c r="B64" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="13" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1970,7 +1976,7 @@
       <c r="B65" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="13" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2009,7 +2015,7 @@
       <c r="B68" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C68" s="13" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2048,7 +2054,7 @@
       <c r="B71" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C71" s="13" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1501.Countries You Can Safely Invest In 可以放心投資的國家
</commit_message>
<xml_diff>
--- a/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
+++ b/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="80">
   <si>
     <t>Easy</t>
   </si>
@@ -913,8 +913,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1968,6 +1968,9 @@
       <c r="C64" s="13" t="s">
         <v>1</v>
       </c>
+      <c r="D64" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="65" spans="1:4" ht="24.95" customHeight="1">
       <c r="A65" s="7">
@@ -1978,6 +1981,9 @@
       </c>
       <c r="C65" s="13" t="s">
         <v>1</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="24.95" hidden="1" customHeight="1">

</xml_diff>

<commit_message>
615.Average Salary: Departments VS Company 平均薪資：部門 VS 公司
</commit_message>
<xml_diff>
--- a/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
+++ b/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="81">
   <si>
     <t>Easy</t>
   </si>
@@ -378,6 +378,10 @@
   </si>
   <si>
     <t>Medium</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -913,8 +917,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -995,7 +999,7 @@
       <c r="R3" s="14"/>
       <c r="S3" s="14"/>
     </row>
-    <row r="4" spans="1:19" ht="24.95" customHeight="1">
+    <row r="4" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A4" s="7">
         <v>534</v>
       </c>
@@ -1024,7 +1028,7 @@
       <c r="R4" s="14"/>
       <c r="S4" s="14"/>
     </row>
-    <row r="5" spans="1:19" ht="24.95" customHeight="1">
+    <row r="5" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A5" s="7">
         <v>550</v>
       </c>
@@ -1053,7 +1057,7 @@
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
     </row>
-    <row r="6" spans="1:19" ht="24.95" customHeight="1">
+    <row r="6" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A6" s="7">
         <v>570</v>
       </c>
@@ -1082,7 +1086,7 @@
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
     </row>
-    <row r="7" spans="1:19" ht="24.95" hidden="1" customHeight="1">
+    <row r="7" spans="1:19" ht="24.95" customHeight="1">
       <c r="A7" s="7">
         <v>571</v>
       </c>
@@ -1091,6 +1095,9 @@
       </c>
       <c r="C7" s="10" t="s">
         <v>2</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -1108,7 +1115,7 @@
       <c r="R7" s="14"/>
       <c r="S7" s="14"/>
     </row>
-    <row r="8" spans="1:19" ht="24.95" customHeight="1">
+    <row r="8" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A8" s="7">
         <v>580</v>
       </c>
@@ -1224,7 +1231,7 @@
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:19" ht="24.95" customHeight="1">
+    <row r="12" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A12" s="7">
         <v>608</v>
       </c>
@@ -1296,7 +1303,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="24.95" hidden="1" customHeight="1">
+    <row r="15" spans="1:19" ht="24.95" customHeight="1">
       <c r="A15" s="7">
         <v>615</v>
       </c>
@@ -1306,8 +1313,11 @@
       <c r="C15" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" ht="24.95" customHeight="1">
+      <c r="D15" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A16" s="7">
         <v>1045</v>
       </c>
@@ -1377,7 +1387,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24.95" customHeight="1">
+    <row r="21" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A21" s="7">
         <v>1077</v>
       </c>
@@ -1433,7 +1443,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="25" spans="1:4" ht="24.95" customHeight="1">
       <c r="A25" s="7">
         <v>1097</v>
       </c>
@@ -1444,7 +1454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="24.95" customHeight="1">
+    <row r="26" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A26" s="7">
         <v>1098</v>
       </c>
@@ -1458,7 +1468,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="24.95" customHeight="1">
+    <row r="27" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A27" s="7">
         <v>1112</v>
       </c>
@@ -1486,7 +1496,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="24.95" customHeight="1">
+    <row r="29" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A29" s="7">
         <v>1126</v>
       </c>
@@ -1500,7 +1510,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="24.95" customHeight="1">
+    <row r="30" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A30" s="7">
         <v>1132</v>
       </c>
@@ -1542,7 +1552,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="24.95" customHeight="1">
+    <row r="33" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A33" s="7">
         <v>1149</v>
       </c>
@@ -1556,7 +1566,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="24.95" customHeight="1">
+    <row r="34" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A34" s="7">
         <v>1164</v>
       </c>
@@ -1584,7 +1594,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24.95" customHeight="1">
+    <row r="36" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A36" s="7">
         <v>1193</v>
       </c>
@@ -1598,7 +1608,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="37" spans="1:4" ht="24.95" customHeight="1">
       <c r="A37" s="7">
         <v>1194</v>
       </c>
@@ -1609,7 +1619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="24.95" customHeight="1">
+    <row r="38" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A38" s="7">
         <v>1204</v>
       </c>
@@ -1623,7 +1633,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="24.95" customHeight="1">
+    <row r="39" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A39" s="7">
         <v>1205</v>
       </c>
@@ -1637,7 +1647,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24.95" customHeight="1">
+    <row r="40" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A40" s="7">
         <v>1212</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="41" spans="1:4" ht="24.95" customHeight="1">
       <c r="A41" s="7">
         <v>1225</v>
       </c>
@@ -1676,7 +1686,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="24.95" customHeight="1">
+    <row r="43" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A43" s="7">
         <v>1264</v>
       </c>
@@ -1690,7 +1700,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="24.95" customHeight="1">
+    <row r="44" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A44" s="7">
         <v>1270</v>
       </c>
@@ -1718,7 +1728,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="24.95" customHeight="1">
+    <row r="46" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A46" s="7">
         <v>1285</v>
       </c>
@@ -1760,7 +1770,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="24.95" customHeight="1">
+    <row r="49" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A49" s="7">
         <v>1308</v>
       </c>
@@ -1774,7 +1784,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="24.95" customHeight="1">
+    <row r="50" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A50" s="7">
         <v>1321</v>
       </c>
@@ -1816,7 +1826,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="53" spans="1:4" ht="24.95" customHeight="1">
       <c r="A53" s="7">
         <v>1336</v>
       </c>
@@ -1827,7 +1837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="24.95" customHeight="1">
+    <row r="54" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A54" s="7">
         <v>1341</v>
       </c>
@@ -1855,7 +1865,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="56" spans="1:4" ht="24.95" customHeight="1">
       <c r="A56" s="7">
         <v>1369</v>
       </c>
@@ -1880,7 +1890,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="58" spans="1:4" ht="24.95" customHeight="1">
       <c r="A58" s="7">
         <v>1384</v>
       </c>
@@ -1891,7 +1901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="24.95" customHeight="1">
+    <row r="59" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A59" s="7">
         <v>1393</v>
       </c>
@@ -1919,7 +1929,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="61" spans="1:4" ht="24.95" customHeight="1">
       <c r="A61" s="7">
         <v>1412</v>
       </c>
@@ -1944,7 +1954,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="24.95" customHeight="1">
+    <row r="63" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A63" s="7">
         <v>1440</v>
       </c>
@@ -1958,7 +1968,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="24.95" customHeight="1">
+    <row r="64" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A64" s="7">
         <v>1445</v>
       </c>
@@ -1972,7 +1982,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="24.95" customHeight="1">
+    <row r="65" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A65" s="7">
         <v>1468</v>
       </c>
@@ -2014,7 +2024,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="24.95" customHeight="1">
+    <row r="68" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A68" s="7">
         <v>1501</v>
       </c>
@@ -2056,7 +2066,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="24.95" customHeight="1">
+    <row r="71" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A71" s="7">
         <v>1532</v>
       </c>
@@ -2065,15 +2075,21 @@
       </c>
       <c r="C71" s="13" t="s">
         <v>1</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C71">
     <filterColumn colId="2">
       <filters>
-        <filter val="Medium"/>
+        <filter val="Hard"/>
       </filters>
     </filterColumn>
+    <sortState ref="A2:C71">
+      <sortCondition ref="A1:A71"/>
+    </sortState>
   </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="E2:S13"/>

</xml_diff>

<commit_message>
1412.Find the Quiet Students in All Exams 查找成績處於中間的學生
</commit_message>
<xml_diff>
--- a/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
+++ b/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="81">
   <si>
     <t>Easy</t>
   </si>
@@ -917,8 +917,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1453,6 +1453,9 @@
       <c r="C25" s="10" t="s">
         <v>2</v>
       </c>
+      <c r="D25" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A26" s="7">
@@ -1618,6 +1621,9 @@
       <c r="C37" s="10" t="s">
         <v>2</v>
       </c>
+      <c r="D37" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A38" s="7">
@@ -1671,6 +1677,9 @@
       <c r="C41" s="10" t="s">
         <v>2</v>
       </c>
+      <c r="D41" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A42" s="7">
@@ -1836,6 +1845,9 @@
       <c r="C53" s="10" t="s">
         <v>2</v>
       </c>
+      <c r="D53" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A54" s="7">
@@ -1875,6 +1887,9 @@
       <c r="C56" s="10" t="s">
         <v>2</v>
       </c>
+      <c r="D56" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A57" s="7">
@@ -1900,6 +1915,9 @@
       <c r="C58" s="10" t="s">
         <v>2</v>
       </c>
+      <c r="D58" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A59" s="7">
@@ -1938,6 +1956,9 @@
       </c>
       <c r="C61" s="10" t="s">
         <v>2</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="24.95" hidden="1" customHeight="1">

</xml_diff>

<commit_message>
LeetCode Curated SQL 70 Medium 29
</commit_message>
<xml_diff>
--- a/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
+++ b/LeetCode_Curated_SQL/LeetCodeSQL.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
   <si>
     <t>Easy</t>
   </si>
@@ -918,7 +918,7 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -949,9 +949,7 @@
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D2" s="11"/>
       <c r="E2" s="14" t="s">
         <v>77</v>
       </c>
@@ -980,9 +978,7 @@
       <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D3" s="11"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -999,7 +995,7 @@
       <c r="R3" s="14"/>
       <c r="S3" s="14"/>
     </row>
-    <row r="4" spans="1:19" ht="24.95" hidden="1" customHeight="1">
+    <row r="4" spans="1:19" ht="24.95" customHeight="1">
       <c r="A4" s="7">
         <v>534</v>
       </c>
@@ -1028,7 +1024,7 @@
       <c r="R4" s="14"/>
       <c r="S4" s="14"/>
     </row>
-    <row r="5" spans="1:19" ht="24.95" hidden="1" customHeight="1">
+    <row r="5" spans="1:19" ht="24.95" customHeight="1">
       <c r="A5" s="7">
         <v>550</v>
       </c>
@@ -1057,7 +1053,7 @@
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
     </row>
-    <row r="6" spans="1:19" ht="24.95" hidden="1" customHeight="1">
+    <row r="6" spans="1:19" ht="24.95" customHeight="1">
       <c r="A6" s="7">
         <v>570</v>
       </c>
@@ -1086,7 +1082,7 @@
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
     </row>
-    <row r="7" spans="1:19" ht="24.95" customHeight="1">
+    <row r="7" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A7" s="7">
         <v>571</v>
       </c>
@@ -1115,7 +1111,7 @@
       <c r="R7" s="14"/>
       <c r="S7" s="14"/>
     </row>
-    <row r="8" spans="1:19" ht="24.95" hidden="1" customHeight="1">
+    <row r="8" spans="1:19" ht="24.95" customHeight="1">
       <c r="A8" s="7">
         <v>580</v>
       </c>
@@ -1154,9 +1150,7 @@
       <c r="C9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D9" s="11"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -1183,9 +1177,7 @@
       <c r="C10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D10" s="11"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -1212,9 +1204,7 @@
       <c r="C11" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D11" s="11"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -1231,7 +1221,7 @@
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:19" ht="24.95" hidden="1" customHeight="1">
+    <row r="12" spans="1:19" ht="24.95" customHeight="1">
       <c r="A12" s="7">
         <v>608</v>
       </c>
@@ -1270,9 +1260,7 @@
       <c r="C13" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D13" s="11"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -1299,11 +1287,9 @@
       <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="24.95" customHeight="1">
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:19" ht="24.95" hidden="1" customHeight="1">
       <c r="A15" s="7">
         <v>615</v>
       </c>
@@ -1317,7 +1303,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="24.95" hidden="1" customHeight="1">
+    <row r="16" spans="1:19" ht="24.95" customHeight="1">
       <c r="A16" s="7">
         <v>1045</v>
       </c>
@@ -1341,9 +1327,7 @@
       <c r="C17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A18" s="7">
@@ -1355,9 +1339,7 @@
       <c r="C18" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A19" s="7">
@@ -1369,9 +1351,7 @@
       <c r="C19" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A20" s="7">
@@ -1383,11 +1363,9 @@
       <c r="C20" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" ht="24.95" customHeight="1">
       <c r="A21" s="7">
         <v>1077</v>
       </c>
@@ -1411,9 +1389,7 @@
       <c r="C22" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A23" s="7">
@@ -1425,9 +1401,7 @@
       <c r="C23" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A24" s="7">
@@ -1439,11 +1413,9 @@
       <c r="C24" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="24.95" customHeight="1">
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A25" s="7">
         <v>1097</v>
       </c>
@@ -1457,7 +1429,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="26" spans="1:4" ht="24.95" customHeight="1">
       <c r="A26" s="7">
         <v>1098</v>
       </c>
@@ -1471,7 +1443,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="27" spans="1:4" ht="24.95" customHeight="1">
       <c r="A27" s="7">
         <v>1112</v>
       </c>
@@ -1495,11 +1467,9 @@
       <c r="C28" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:4" ht="24.95" customHeight="1">
       <c r="A29" s="7">
         <v>1126</v>
       </c>
@@ -1513,7 +1483,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="30" spans="1:4" ht="24.95" customHeight="1">
       <c r="A30" s="7">
         <v>1132</v>
       </c>
@@ -1537,9 +1507,7 @@
       <c r="C31" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A32" s="7">
@@ -1551,11 +1519,9 @@
       <c r="C32" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" ht="24.95" customHeight="1">
       <c r="A33" s="7">
         <v>1149</v>
       </c>
@@ -1569,7 +1535,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="34" spans="1:4" ht="24.95" customHeight="1">
       <c r="A34" s="7">
         <v>1164</v>
       </c>
@@ -1593,11 +1559,9 @@
       <c r="C35" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="24.95" customHeight="1">
       <c r="A36" s="7">
         <v>1193</v>
       </c>
@@ -1611,7 +1575,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="24.95" customHeight="1">
+    <row r="37" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A37" s="7">
         <v>1194</v>
       </c>
@@ -1625,7 +1589,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="38" spans="1:4" ht="24.95" customHeight="1">
       <c r="A38" s="7">
         <v>1204</v>
       </c>
@@ -1639,7 +1603,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="39" spans="1:4" ht="24.95" customHeight="1">
       <c r="A39" s="7">
         <v>1205</v>
       </c>
@@ -1653,7 +1617,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="40" spans="1:4" ht="24.95" customHeight="1">
       <c r="A40" s="7">
         <v>1212</v>
       </c>
@@ -1667,7 +1631,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="24.95" customHeight="1">
+    <row r="41" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A41" s="7">
         <v>1225</v>
       </c>
@@ -1691,11 +1655,9 @@
       <c r="C42" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" ht="24.95" customHeight="1">
       <c r="A43" s="7">
         <v>1264</v>
       </c>
@@ -1709,7 +1671,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="44" spans="1:4" ht="24.95" customHeight="1">
       <c r="A44" s="7">
         <v>1270</v>
       </c>
@@ -1733,11 +1695,9 @@
       <c r="C45" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="1:4" ht="24.95" customHeight="1">
       <c r="A46" s="7">
         <v>1285</v>
       </c>
@@ -1761,9 +1721,7 @@
       <c r="C47" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A48" s="7">
@@ -1775,11 +1733,9 @@
       <c r="C48" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D48" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="1:4" ht="24.95" customHeight="1">
       <c r="A49" s="7">
         <v>1308</v>
       </c>
@@ -1793,7 +1749,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="50" spans="1:4" ht="24.95" customHeight="1">
       <c r="A50" s="7">
         <v>1321</v>
       </c>
@@ -1817,9 +1773,7 @@
       <c r="C51" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A52" s="7">
@@ -1831,11 +1785,9 @@
       <c r="C52" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="24.95" customHeight="1">
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A53" s="7">
         <v>1336</v>
       </c>
@@ -1849,7 +1801,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="54" spans="1:4" ht="24.95" customHeight="1">
       <c r="A54" s="7">
         <v>1341</v>
       </c>
@@ -1873,11 +1825,9 @@
       <c r="C55" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D55" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="24.95" customHeight="1">
+      <c r="D55" s="11"/>
+    </row>
+    <row r="56" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A56" s="7">
         <v>1369</v>
       </c>
@@ -1901,11 +1851,9 @@
       <c r="C57" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D57" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="24.95" customHeight="1">
+      <c r="D57" s="11"/>
+    </row>
+    <row r="58" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A58" s="7">
         <v>1384</v>
       </c>
@@ -1919,7 +1867,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="59" spans="1:4" ht="24.95" customHeight="1">
       <c r="A59" s="7">
         <v>1393</v>
       </c>
@@ -1943,11 +1891,9 @@
       <c r="C60" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D60" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="24.95" customHeight="1">
+      <c r="D60" s="11"/>
+    </row>
+    <row r="61" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A61" s="7">
         <v>1412</v>
       </c>
@@ -1971,11 +1917,9 @@
       <c r="C62" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D62" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D62" s="11"/>
+    </row>
+    <row r="63" spans="1:4" ht="24.95" customHeight="1">
       <c r="A63" s="7">
         <v>1440</v>
       </c>
@@ -1989,7 +1933,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="64" spans="1:4" ht="24.95" customHeight="1">
       <c r="A64" s="7">
         <v>1445</v>
       </c>
@@ -2003,7 +1947,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="65" spans="1:4" ht="24.95" customHeight="1">
       <c r="A65" s="7">
         <v>1468</v>
       </c>
@@ -2027,9 +1971,7 @@
       <c r="C66" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D66" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A67" s="7">
@@ -2041,11 +1983,9 @@
       <c r="C67" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D67" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D67" s="11"/>
+    </row>
+    <row r="68" spans="1:4" ht="24.95" customHeight="1">
       <c r="A68" s="7">
         <v>1501</v>
       </c>
@@ -2069,9 +2009,7 @@
       <c r="C69" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D69" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="D69" s="11"/>
     </row>
     <row r="70" spans="1:4" ht="24.95" hidden="1" customHeight="1">
       <c r="A70" s="7">
@@ -2083,11 +2021,9 @@
       <c r="C70" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D70" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="D70" s="11"/>
+    </row>
+    <row r="71" spans="1:4" ht="24.95" customHeight="1">
       <c r="A71" s="7">
         <v>1532</v>
       </c>
@@ -2105,7 +2041,7 @@
   <autoFilter ref="A1:C71">
     <filterColumn colId="2">
       <filters>
-        <filter val="Hard"/>
+        <filter val="Medium"/>
       </filters>
     </filterColumn>
     <sortState ref="A2:C71">

</xml_diff>